<commit_message>
some model parameters for Picea abies
</commit_message>
<xml_diff>
--- a/software/3D-CMCC-Forest-Model/input/AUZobelboden/doc/IP1_Soil.xlsx
+++ b/software/3D-CMCC-Forest-Model/input/AUZobelboden/doc/IP1_Soil.xlsx
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Alessio</author>
+  </authors>
+  <commentList>
+    <comment ref="M25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Alessio:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+poiché la somma non è 100 aggiundo a ciascuno +1</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="84">
   <si>
     <t xml:space="preserve">pH </t>
   </si>
@@ -268,12 +302,6 @@
   </si>
   <si>
     <t>Alessio</t>
-  </si>
-  <si>
-    <t>media su tutti</t>
-  </si>
-  <si>
-    <t>tot</t>
   </si>
 </sst>
 </file>
@@ -284,7 +312,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +340,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -477,6 +518,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -513,10 +558,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -819,7 +860,7 @@
   <dimension ref="A1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -831,21 +872,21 @@
     <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="38"/>
+    <col min="12" max="12" width="11.42578125" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="L1" s="38" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="L1" s="26" t="s">
         <v>83</v>
       </c>
     </row>
@@ -918,7 +959,7 @@
       </c>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="30" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -942,13 +983,13 @@
       <c r="H5" s="11">
         <v>2.2569256072745909</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="27">
         <f>AVERAGE(D5:H5)</f>
         <v>2.919803145826152</v>
       </c>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="26"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
@@ -970,13 +1011,13 @@
       <c r="H6" s="11">
         <v>54.845263605050626</v>
       </c>
-      <c r="L6" s="39">
+      <c r="L6" s="27">
         <f>AVERAGE(D6:H6)</f>
         <v>59.78243522940916</v>
       </c>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="26"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
@@ -998,7 +1039,7 @@
       <c r="H7" s="11">
         <v>42.897810787674786</v>
       </c>
-      <c r="L7" s="39">
+      <c r="L7" s="27">
         <f>AVERAGE(D7:H7)</f>
         <v>37.297639231518637</v>
       </c>
@@ -1024,7 +1065,7 @@
       <c r="H8" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="L8" s="39">
+      <c r="L8" s="27">
         <f>SUM(L5:L7)</f>
         <v>99.999877606753955</v>
       </c>
@@ -1048,7 +1089,7 @@
       <c r="H9" s="21">
         <v>0</v>
       </c>
-      <c r="L9" s="38"/>
+      <c r="L9" s="26"/>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" t="s">
@@ -1072,9 +1113,9 @@
       <c r="H10" s="5">
         <v>1.1302894826495564</v>
       </c>
-      <c r="L10" s="40">
-        <f>AVERAGE(C10:H10)</f>
-        <v>0.70721865111530224</v>
+      <c r="L10" s="28">
+        <f>AVERAGE(D10:H10)</f>
+        <v>0.82783810010379477</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1102,18 +1143,18 @@
       <c r="A12" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="33">
+      <c r="E12" s="33"/>
+      <c r="F12" s="37">
         <v>57</v>
       </c>
-      <c r="G12" s="33"/>
+      <c r="G12" s="37"/>
       <c r="H12">
         <v>58</v>
       </c>
-      <c r="L12" s="41">
+      <c r="L12" s="29">
         <f>AVERAGE(D12:H12)</f>
         <v>57.5</v>
       </c>
@@ -1122,18 +1163,18 @@
       <c r="A13" t="s">
         <v>78</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="32">
+      <c r="E13" s="35"/>
+      <c r="F13" s="36">
         <v>45</v>
       </c>
-      <c r="G13" s="32"/>
+      <c r="G13" s="36"/>
       <c r="H13">
         <v>47</v>
       </c>
-      <c r="L13" s="41">
+      <c r="L13" s="29">
         <f>AVERAGE(D13:H13)</f>
         <v>46</v>
       </c>
@@ -1253,16 +1294,16 @@
       <c r="H19" s="6"/>
     </row>
     <row r="21" spans="1:16">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
     </row>
     <row r="22" spans="1:16">
       <c r="C22" t="s">
@@ -1331,12 +1372,9 @@
       <c r="H24" s="3">
         <v>20</v>
       </c>
-      <c r="P24" t="s">
-        <v>84</v>
-      </c>
     </row>
     <row r="25" spans="1:16">
-      <c r="A25" s="26" t="s">
+      <c r="A25" s="30" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1360,20 +1398,18 @@
       <c r="H25" s="11">
         <v>3.5240284140330398</v>
       </c>
-      <c r="L25" s="39">
+      <c r="L25" s="27">
         <f>AVERAGE(D25:H25)</f>
         <v>8.9702056270753729</v>
       </c>
-      <c r="O25" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P25" s="9">
-        <f>AVERAGE(D5:H5,D25:H25,D45:H45)</f>
-        <v>11.792195054147092</v>
-      </c>
+      <c r="M25">
+        <v>10</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="9"/>
     </row>
     <row r="26" spans="1:16">
-      <c r="A26" s="26"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
@@ -1395,20 +1431,18 @@
       <c r="H26" s="11">
         <v>57.293625186596529</v>
       </c>
-      <c r="L26" s="39">
+      <c r="L26" s="27">
         <f>AVERAGE(D26:H26)</f>
         <v>50.346989019932053</v>
       </c>
-      <c r="O26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P26" s="9">
-        <f>AVERAGE(D6:H6,D26:H26,D46:H46)</f>
-        <v>54.224415265395365</v>
-      </c>
+      <c r="M26">
+        <v>51</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="9"/>
     </row>
     <row r="27" spans="1:16">
-      <c r="A27" s="26"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="2" t="s">
         <v>12</v>
       </c>
@@ -1430,17 +1464,15 @@
       <c r="H27" s="11">
         <v>39.182346399370431</v>
       </c>
-      <c r="L27" s="39">
+      <c r="L27" s="27">
         <f>AVERAGE(D27:H27)</f>
         <v>38.178708518634764</v>
       </c>
-      <c r="O27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P27" s="9">
-        <f>AVERAGE(D7:H7,D27:H27,D47:H47)</f>
-        <v>33.089025670599014</v>
-      </c>
+      <c r="M27">
+        <v>39</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="9"/>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="8" t="s">
@@ -1463,17 +1495,16 @@
       <c r="H28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="L28" s="39">
+      <c r="L28" s="27">
         <f>SUM(L25:L27)</f>
         <v>97.49590316564219</v>
       </c>
-      <c r="O28" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="P28" s="9">
-        <f>SUM(P25:P27)</f>
-        <v>99.105635990141465</v>
-      </c>
+      <c r="M28" s="27">
+        <f>SUM(M25:M27)</f>
+        <v>100</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="9"/>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="12" t="s">
@@ -1509,9 +1540,9 @@
       <c r="H30" s="5">
         <v>1.2030797821332966</v>
       </c>
-      <c r="L30" s="40">
-        <f>AVERAGE(C30:H30)</f>
-        <v>0.79983784767470167</v>
+      <c r="L30" s="28">
+        <f>AVERAGE(D30:H30)</f>
+        <v>0.9442731936911235</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -1541,67 +1572,49 @@
         <f>300/3600</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="O31" t="s">
-        <v>9</v>
-      </c>
-      <c r="P31" s="5">
-        <f>AVERAGE(D10:H10,D30:H30,D50:G50)</f>
-        <v>0.7828404548884117</v>
-      </c>
+      <c r="P31" s="5"/>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="28" t="s">
+      <c r="D32" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="E32" s="29"/>
-      <c r="F32" s="33">
+      <c r="E32" s="33"/>
+      <c r="F32" s="37">
         <v>57</v>
       </c>
-      <c r="G32" s="33"/>
+      <c r="G32" s="37"/>
       <c r="H32" s="25">
         <v>58</v>
       </c>
-      <c r="L32" s="41">
+      <c r="L32" s="29">
         <f>AVERAGE(D32:H32)</f>
         <v>57.5</v>
       </c>
-      <c r="O32" t="s">
-        <v>77</v>
-      </c>
-      <c r="P32" s="10">
-        <f>AVERAGE(D12:H12,D32:H32,D52:G52)</f>
-        <v>52.75</v>
-      </c>
+      <c r="P32" s="10"/>
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="32">
+      <c r="E33" s="35"/>
+      <c r="F33" s="36">
         <v>45</v>
       </c>
-      <c r="G33" s="32"/>
+      <c r="G33" s="36"/>
       <c r="H33" s="25">
         <v>47</v>
       </c>
-      <c r="L33" s="41">
+      <c r="L33" s="29">
         <f>AVERAGE(D33:H33)</f>
         <v>46</v>
       </c>
-      <c r="O33" t="s">
-        <v>78</v>
-      </c>
-      <c r="P33" s="10">
-        <f>AVERAGE(D13:H13,D33:H33,D53:G53)</f>
-        <v>34.25</v>
-      </c>
+      <c r="P33" s="10"/>
     </row>
     <row r="34" spans="1:16">
       <c r="A34" t="s">
@@ -1718,16 +1731,16 @@
       <c r="H39" s="6"/>
     </row>
     <row r="41" spans="1:16">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
     </row>
     <row r="42" spans="1:16">
       <c r="C42" t="s">
@@ -1794,7 +1807,7 @@
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:16">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="30" t="s">
         <v>3</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1816,13 +1829,13 @@
         <v>19.51210597781089</v>
       </c>
       <c r="H45" s="2"/>
-      <c r="L45" s="39">
+      <c r="L45" s="27">
         <f>AVERAGE(D45:G45)</f>
         <v>26.410171723387919</v>
       </c>
     </row>
     <row r="46" spans="1:16">
-      <c r="A46" s="26"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="2" t="s">
         <v>13</v>
       </c>
@@ -1842,13 +1855,13 @@
         <v>53.706795996025832</v>
       </c>
       <c r="H46" s="2"/>
-      <c r="L46" s="39">
+      <c r="L46" s="27">
         <f>AVERAGE(D46:G46)</f>
         <v>52.123673117207275</v>
       </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="26"/>
+      <c r="A47" s="30"/>
       <c r="B47" s="2" t="s">
         <v>12</v>
       </c>
@@ -1868,7 +1881,7 @@
         <v>26.781098026163278</v>
       </c>
       <c r="H47" s="2"/>
-      <c r="L47" s="39">
+      <c r="L47" s="27">
         <f>AVERAGE(D47:G47)</f>
         <v>21.466155159404806</v>
       </c>
@@ -1892,7 +1905,7 @@
         <v>64</v>
       </c>
       <c r="H48" s="2"/>
-      <c r="L48" s="39">
+      <c r="L48" s="27">
         <f>SUM(L45:L47)</f>
         <v>100</v>
       </c>
@@ -1934,6 +1947,10 @@
       <c r="G50" s="5">
         <v>0.82143229002582208</v>
       </c>
+      <c r="L50" s="28">
+        <f>AVERAGE(D50:G50)</f>
+        <v>0.52480247486579301</v>
+      </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" t="s">
@@ -1968,7 +1985,7 @@
       <c r="G52" s="9">
         <v>40</v>
       </c>
-      <c r="L52" s="39">
+      <c r="L52" s="27">
         <f>AVERAGE(D52:G52)</f>
         <v>48</v>
       </c>
@@ -1989,7 +2006,7 @@
       <c r="G53" s="9">
         <v>22</v>
       </c>
-      <c r="L53" s="39">
+      <c r="L53" s="27">
         <f>AVERAGE(D53:G53)</f>
         <v>22.5</v>
       </c>
@@ -2116,6 +2133,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2895,14 +2913,14 @@
       </c>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="34"/>
-      <c r="E25" s="34"/>
-      <c r="F25" s="34"/>
+      <c r="B25" s="38"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" thickBot="1">
       <c r="H26" t="s">
@@ -2926,13 +2944,13 @@
     </row>
     <row r="27" spans="1:17" ht="15.75" thickBot="1">
       <c r="A27" s="15"/>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="37"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41"/>
       <c r="H27" t="s">
         <v>35</v>
       </c>
@@ -3051,12 +3069,12 @@
       <c r="I30" t="s">
         <v>27</v>
       </c>
-      <c r="J30" s="31" t="s">
+      <c r="J30" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="31"/>
+      <c r="K30" s="35"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="35"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" thickBot="1">
       <c r="A31" s="16" t="s">
@@ -3100,13 +3118,13 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" thickBot="1">
       <c r="A33" s="15"/>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="37"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="9"/>
       <c r="H33" t="s">
         <v>35</v>
@@ -3228,12 +3246,12 @@
       <c r="I36" t="s">
         <v>25</v>
       </c>
-      <c r="J36" s="31" t="s">
+      <c r="J36" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
+      <c r="K36" s="35"/>
+      <c r="L36" s="35"/>
+      <c r="M36" s="35"/>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1">
       <c r="A37" s="16" t="s">
@@ -3280,13 +3298,13 @@
     </row>
     <row r="39" spans="1:13" ht="15.75" thickBot="1">
       <c r="A39" s="15"/>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="37"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
       <c r="G39" s="9"/>
       <c r="H39" t="s">
         <v>35</v>
@@ -3425,14 +3443,14 @@
       <c r="G43" s="9"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="34"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="34"/>
-      <c r="E45" s="34"/>
-      <c r="F45" s="34"/>
+      <c r="B45" s="38"/>
+      <c r="C45" s="38"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="38"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1">
       <c r="F46" s="6"/>
@@ -3440,13 +3458,13 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" thickBot="1">
       <c r="A47" s="15"/>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="37"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="41"/>
       <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1">
@@ -3531,13 +3549,13 @@
     <row r="52" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="53" spans="1:6" ht="15.75" thickBot="1">
       <c r="A53" s="15"/>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="37"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="41"/>
     </row>
     <row r="54" spans="1:6" ht="15.75" thickBot="1">
       <c r="A54" s="16"/>
@@ -3620,13 +3638,13 @@
     <row r="58" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="59" spans="1:6" ht="15.75" thickBot="1">
       <c r="A59" s="15"/>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="37"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="41"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" thickBot="1">
       <c r="A60" s="16"/>
@@ -3707,25 +3725,25 @@
       </c>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="34" t="s">
+      <c r="A65" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="67" spans="1:6" ht="15.75" thickBot="1">
       <c r="A67" s="15"/>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="37"/>
+      <c r="C67" s="40"/>
+      <c r="D67" s="40"/>
+      <c r="E67" s="40"/>
+      <c r="F67" s="41"/>
     </row>
     <row r="68" spans="1:6" ht="15.75" thickBot="1">
       <c r="A68" s="16"/>
@@ -3808,13 +3826,13 @@
     <row r="72" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="73" spans="1:6" ht="15.75" thickBot="1">
       <c r="A73" s="15"/>
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C73" s="36"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="37"/>
+      <c r="C73" s="40"/>
+      <c r="D73" s="40"/>
+      <c r="E73" s="40"/>
+      <c r="F73" s="41"/>
     </row>
     <row r="74" spans="1:6" ht="15.75" thickBot="1">
       <c r="A74" s="16"/>
@@ -3897,13 +3915,13 @@
     <row r="78" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="79" spans="1:6" ht="15.75" thickBot="1">
       <c r="A79" s="15"/>
-      <c r="B79" s="35" t="s">
+      <c r="B79" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="C79" s="36"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="37"/>
+      <c r="C79" s="40"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
+      <c r="F79" s="41"/>
     </row>
     <row r="80" spans="1:6" ht="15.75" thickBot="1">
       <c r="A80" s="16"/>
@@ -3984,25 +4002,25 @@
       </c>
     </row>
     <row r="85" spans="1:6">
-      <c r="A85" s="34" t="s">
+      <c r="A85" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B85" s="34"/>
-      <c r="C85" s="34"/>
-      <c r="D85" s="34"/>
-      <c r="E85" s="34"/>
-      <c r="F85" s="34"/>
+      <c r="B85" s="38"/>
+      <c r="C85" s="38"/>
+      <c r="D85" s="38"/>
+      <c r="E85" s="38"/>
+      <c r="F85" s="38"/>
     </row>
     <row r="86" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="87" spans="1:6" ht="15.75" thickBot="1">
       <c r="A87" s="15"/>
-      <c r="B87" s="35" t="s">
+      <c r="B87" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="C87" s="36"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="37"/>
+      <c r="C87" s="40"/>
+      <c r="D87" s="40"/>
+      <c r="E87" s="40"/>
+      <c r="F87" s="41"/>
     </row>
     <row r="88" spans="1:6" ht="15.75" thickBot="1">
       <c r="A88" s="16"/>
@@ -4085,13 +4103,13 @@
     <row r="92" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="93" spans="1:6" ht="15.75" thickBot="1">
       <c r="A93" s="15"/>
-      <c r="B93" s="35" t="s">
+      <c r="B93" s="39" t="s">
         <v>61</v>
       </c>
-      <c r="C93" s="36"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
-      <c r="F93" s="37"/>
+      <c r="C93" s="40"/>
+      <c r="D93" s="40"/>
+      <c r="E93" s="40"/>
+      <c r="F93" s="41"/>
     </row>
     <row r="94" spans="1:6" ht="15.75" thickBot="1">
       <c r="A94" s="16"/>
@@ -4174,13 +4192,13 @@
     <row r="98" spans="1:6" ht="15.75" thickBot="1"/>
     <row r="99" spans="1:6" ht="15.75" thickBot="1">
       <c r="A99" s="15"/>
-      <c r="B99" s="35" t="s">
+      <c r="B99" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C99" s="36"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="37"/>
+      <c r="C99" s="40"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="40"/>
+      <c r="F99" s="41"/>
     </row>
     <row r="100" spans="1:6" ht="15.75" thickBot="1">
       <c r="A100" s="16"/>
@@ -4261,20 +4279,20 @@
       </c>
     </row>
     <row r="105" spans="1:6">
-      <c r="A105" s="34"/>
-      <c r="B105" s="34"/>
-      <c r="C105" s="34"/>
-      <c r="D105" s="34"/>
-      <c r="E105" s="34"/>
-      <c r="F105" s="34"/>
+      <c r="A105" s="38"/>
+      <c r="B105" s="38"/>
+      <c r="C105" s="38"/>
+      <c r="D105" s="38"/>
+      <c r="E105" s="38"/>
+      <c r="F105" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="A45:F45"/>
-    <mergeCell ref="B67:F67"/>
-    <mergeCell ref="B73:F73"/>
+    <mergeCell ref="A85:F85"/>
+    <mergeCell ref="B87:F87"/>
+    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B99:F99"/>
+    <mergeCell ref="A105:F105"/>
     <mergeCell ref="B79:F79"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B33:F33"/>
@@ -4284,11 +4302,11 @@
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="B59:F59"/>
     <mergeCell ref="A65:F65"/>
-    <mergeCell ref="A85:F85"/>
-    <mergeCell ref="B87:F87"/>
-    <mergeCell ref="B93:F93"/>
-    <mergeCell ref="B99:F99"/>
-    <mergeCell ref="A105:F105"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="B47:F47"/>
+    <mergeCell ref="A45:F45"/>
+    <mergeCell ref="B67:F67"/>
+    <mergeCell ref="B73:F73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>